<commit_message>
ajout définition élément location
ajout définition élément location d183af69a8590856ba04be8bb57765ad18b65c80
</commit_message>
<xml_diff>
--- a/ig/sd-pays-de-recrutement/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-pays-de-recrutement/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-27T08:07:53+00:00</t>
+    <t>2023-07-27T08:11:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1094,7 +1094,7 @@
     <t>ResearchStudy.location</t>
   </si>
   <si>
-    <t>Geographic region(s) for study</t>
+    <t>Pays de recrutement / Countries of Recruitment</t>
   </si>
   <si>
     <t>Indicates a country, state or other region where the study is taking place.</t>
@@ -1194,7 +1194,7 @@
     <t>ResearchStudy.sponsor</t>
   </si>
   <si>
-    <t>promoteur / primary Sponsor</t>
+    <t>Promoteur / primary Sponsor</t>
   </si>
   <si>
     <t>An organization that initiates the investigation and is legally responsible for the study.</t>

</xml_diff>